<commit_message>
feat: Published NHS Equity and Skin Tone standards
</commit_message>
<xml_diff>
--- a/docs/observations-summary.xlsx
+++ b/docs/observations-summary.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="31">
   <si>
     <t>Profile</t>
   </si>
@@ -53,7 +53,7 @@
     <t>Open Nursing Core Braden Scale Assessment</t>
   </si>
   <si>
-    <t>null#nursing</t>
+    <t>Observation Category Codes#nursing</t>
   </si>
   <si>
     <t/>
@@ -93,6 +93,18 @@
   </si>
   <si>
     <t>http://hl7.org/fhir/ValueSet/observation-codes|4.0.1 (example)</t>
+  </si>
+  <si>
+    <t>onc-skintone-observation</t>
+  </si>
+  <si>
+    <t>ONC Skin Tone Observation</t>
+  </si>
+  <si>
+    <t>LOINC#66472-2</t>
+  </si>
+  <si>
+    <t>CodeableConceptĵ</t>
   </si>
 </sst>
 </file>
@@ -226,7 +238,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:K10"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -582,6 +594,41 @@
         <v>14</v>
       </c>
     </row>
+    <row r="11">
+      <c r="A11" t="s" s="2">
+        <v>27</v>
+      </c>
+      <c r="B11" t="s" s="2">
+        <v>28</v>
+      </c>
+      <c r="C11" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="D11" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="E11" t="s" s="2">
+        <v>29</v>
+      </c>
+      <c r="F11" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="G11" t="s" s="2">
+        <v>16</v>
+      </c>
+      <c r="H11" t="s" s="2">
+        <v>30</v>
+      </c>
+      <c r="I11" t="s" s="2">
+        <v>18</v>
+      </c>
+      <c r="J11" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="K11" t="s" s="2">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
fix: Resolved terminology and configuration errors
</commit_message>
<xml_diff>
--- a/docs/observations-summary.xlsx
+++ b/docs/observations-summary.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="55">
   <si>
     <t>Profile</t>
   </si>
@@ -86,6 +86,81 @@
     <t>Quantityĵ, CodeableConceptĵ</t>
   </si>
   <si>
+    <t>onc-housing-status</t>
+  </si>
+  <si>
+    <t>ONC Housing Status Assessment</t>
+  </si>
+  <si>
+    <t>LOINC#71802-3</t>
+  </si>
+  <si>
+    <t>CodeableConceptĵ</t>
+  </si>
+  <si>
+    <t>onc-morse-fall-scale</t>
+  </si>
+  <si>
+    <t>ONC Morse Fall Scale Assessment</t>
+  </si>
+  <si>
+    <t>LOINC#59460-6</t>
+  </si>
+  <si>
+    <t>LOINC#59461-4</t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>LOINC#59462-2</t>
+  </si>
+  <si>
+    <t>LOINC#59463-0</t>
+  </si>
+  <si>
+    <t>LOINC#59464-8</t>
+  </si>
+  <si>
+    <t>LOINC#59465-5</t>
+  </si>
+  <si>
+    <t>LOINC#59466-3</t>
+  </si>
+  <si>
+    <t>onc-news2-assessment</t>
+  </si>
+  <si>
+    <t>ONC NEWS2 Assessment</t>
+  </si>
+  <si>
+    <t>LOINC#86585-7</t>
+  </si>
+  <si>
+    <t>LOINC#9279-1</t>
+  </si>
+  <si>
+    <t>LOINC#2708-6</t>
+  </si>
+  <si>
+    <t>LOINC#8310-5</t>
+  </si>
+  <si>
+    <t>LOINC#8480-6</t>
+  </si>
+  <si>
+    <t>LOINC#8867-4</t>
+  </si>
+  <si>
+    <t>LOINC#11454-5</t>
+  </si>
+  <si>
+    <t>CodeableConcept</t>
+  </si>
+  <si>
+    <t>LOINC#72274-4</t>
+  </si>
+  <si>
     <t>onc-nursing-assessment</t>
   </si>
   <si>
@@ -102,9 +177,6 @@
   </si>
   <si>
     <t>LOINC#66472-2</t>
-  </si>
-  <si>
-    <t>CodeableConceptĵ</t>
   </si>
 </sst>
 </file>
@@ -238,7 +310,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:K11"/>
+  <dimension ref="A1:K27"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -573,16 +645,16 @@
         <v>14</v>
       </c>
       <c r="E10" t="s" s="2">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="F10" t="s" s="2">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="G10" t="s" s="2">
         <v>16</v>
       </c>
       <c r="H10" t="s" s="2">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="I10" t="s" s="2">
         <v>18</v>
@@ -596,19 +668,19 @@
     </row>
     <row r="11">
       <c r="A11" t="s" s="2">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B11" t="s" s="2">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C11" t="s" s="2">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D11" t="s" s="2">
         <v>14</v>
       </c>
       <c r="E11" t="s" s="2">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F11" t="s" s="2">
         <v>14</v>
@@ -617,7 +689,7 @@
         <v>16</v>
       </c>
       <c r="H11" t="s" s="2">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="I11" t="s" s="2">
         <v>18</v>
@@ -626,6 +698,566 @@
         <v>14</v>
       </c>
       <c r="K11" t="s" s="2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="B12" t="s" s="2">
+        <v>29</v>
+      </c>
+      <c r="C12" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="D12" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="E12" t="s" s="2">
+        <v>31</v>
+      </c>
+      <c r="F12" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="G12" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="H12" t="s" s="2">
+        <v>32</v>
+      </c>
+      <c r="I12" t="s" s="2">
+        <v>18</v>
+      </c>
+      <c r="J12" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="K12" t="s" s="2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="B13" t="s" s="2">
+        <v>29</v>
+      </c>
+      <c r="C13" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="D13" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="E13" t="s" s="2">
+        <v>33</v>
+      </c>
+      <c r="F13" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="G13" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="H13" t="s" s="2">
+        <v>32</v>
+      </c>
+      <c r="I13" t="s" s="2">
+        <v>18</v>
+      </c>
+      <c r="J13" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="K13" t="s" s="2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="B14" t="s" s="2">
+        <v>29</v>
+      </c>
+      <c r="C14" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="D14" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="E14" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="F14" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="G14" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="H14" t="s" s="2">
+        <v>32</v>
+      </c>
+      <c r="I14" t="s" s="2">
+        <v>18</v>
+      </c>
+      <c r="J14" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="K14" t="s" s="2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s" s="2">
+        <v>29</v>
+      </c>
+      <c r="C15" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="D15" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="E15" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="F15" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="G15" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="H15" t="s" s="2">
+        <v>32</v>
+      </c>
+      <c r="I15" t="s" s="2">
+        <v>18</v>
+      </c>
+      <c r="J15" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="K15" t="s" s="2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s" s="2">
+        <v>29</v>
+      </c>
+      <c r="C16" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="D16" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="E16" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="F16" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="G16" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="H16" t="s" s="2">
+        <v>32</v>
+      </c>
+      <c r="I16" t="s" s="2">
+        <v>18</v>
+      </c>
+      <c r="J16" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="K16" t="s" s="2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="B17" t="s" s="2">
+        <v>29</v>
+      </c>
+      <c r="C17" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="D17" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="E17" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="F17" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="G17" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="H17" t="s" s="2">
+        <v>32</v>
+      </c>
+      <c r="I17" t="s" s="2">
+        <v>18</v>
+      </c>
+      <c r="J17" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="K17" t="s" s="2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="B18" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="C18" t="s" s="2">
+        <v>13</v>
+      </c>
+      <c r="D18" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="E18" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="F18" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="G18" t="s" s="2">
+        <v>16</v>
+      </c>
+      <c r="H18" t="s" s="2">
+        <v>17</v>
+      </c>
+      <c r="I18" t="s" s="2">
+        <v>18</v>
+      </c>
+      <c r="J18" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="K18" t="s" s="2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="B19" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="C19" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="D19" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="E19" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="F19" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="G19" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="H19" t="s" s="2">
+        <v>32</v>
+      </c>
+      <c r="I19" t="s" s="2">
+        <v>18</v>
+      </c>
+      <c r="J19" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="K19" t="s" s="2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="B20" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="C20" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="D20" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="E20" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="F20" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="G20" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="H20" t="s" s="2">
+        <v>32</v>
+      </c>
+      <c r="I20" t="s" s="2">
+        <v>18</v>
+      </c>
+      <c r="J20" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="K20" t="s" s="2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="B21" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="C21" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="D21" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="E21" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="F21" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="G21" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="H21" t="s" s="2">
+        <v>32</v>
+      </c>
+      <c r="I21" t="s" s="2">
+        <v>18</v>
+      </c>
+      <c r="J21" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="K21" t="s" s="2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="B22" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="C22" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="D22" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="E22" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="F22" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="G22" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="H22" t="s" s="2">
+        <v>32</v>
+      </c>
+      <c r="I22" t="s" s="2">
+        <v>18</v>
+      </c>
+      <c r="J22" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="K22" t="s" s="2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="B23" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="C23" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="D23" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="E23" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="F23" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="G23" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="H23" t="s" s="2">
+        <v>32</v>
+      </c>
+      <c r="I23" t="s" s="2">
+        <v>18</v>
+      </c>
+      <c r="J23" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="K23" t="s" s="2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="B24" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="C24" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="D24" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="E24" t="s" s="2">
+        <v>46</v>
+      </c>
+      <c r="F24" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="G24" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="H24" t="s" s="2">
+        <v>47</v>
+      </c>
+      <c r="I24" t="s" s="2">
+        <v>18</v>
+      </c>
+      <c r="J24" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="K24" t="s" s="2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="B25" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="C25" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="D25" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="E25" t="s" s="2">
+        <v>48</v>
+      </c>
+      <c r="F25" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="G25" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="H25" t="s" s="2">
+        <v>47</v>
+      </c>
+      <c r="I25" t="s" s="2">
+        <v>18</v>
+      </c>
+      <c r="J25" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="K25" t="s" s="2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s" s="2">
+        <v>49</v>
+      </c>
+      <c r="B26" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="C26" t="s" s="2">
+        <v>13</v>
+      </c>
+      <c r="D26" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="E26" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="F26" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="G26" t="s" s="2">
+        <v>16</v>
+      </c>
+      <c r="H26" t="s" s="2">
+        <v>23</v>
+      </c>
+      <c r="I26" t="s" s="2">
+        <v>18</v>
+      </c>
+      <c r="J26" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="K26" t="s" s="2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s" s="2">
+        <v>52</v>
+      </c>
+      <c r="B27" t="s" s="2">
+        <v>53</v>
+      </c>
+      <c r="C27" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="D27" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="E27" t="s" s="2">
+        <v>54</v>
+      </c>
+      <c r="F27" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="G27" t="s" s="2">
+        <v>16</v>
+      </c>
+      <c r="H27" t="s" s="2">
+        <v>27</v>
+      </c>
+      <c r="I27" t="s" s="2">
+        <v>18</v>
+      </c>
+      <c r="J27" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="K27" t="s" s="2">
         <v>14</v>
       </c>
     </row>

</xml_diff>